<commit_message>
BD estable sin restriciones
</commit_message>
<xml_diff>
--- a/WebContent/acciones usuario.xlsx
+++ b/WebContent/acciones usuario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>B  : Baja</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>ver PrecioHoras</t>
+  </si>
+  <si>
+    <t>iniciar sesión</t>
   </si>
 </sst>
 </file>
@@ -706,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1412,9 @@
       <c r="A76" t="s">
         <v>62</v>
       </c>
-      <c r="B76" s="1"/>
+      <c r="B76" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
         <v>53</v>
@@ -1429,7 +1434,9 @@
       <c r="A78" t="s">
         <v>63</v>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
         <v>53</v>
@@ -1466,7 +1473,12 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
+      <c r="A82" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>

</xml_diff>